<commit_message>
blank spreadsheet invoice data
</commit_message>
<xml_diff>
--- a/src/python/invoice_data.xlsx
+++ b/src/python/invoice_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dalton/Code/cohort3/src/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24017976-4AE3-9E4C-BB0F-51FA8DD7C9D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA3A5CB-BFF1-D248-904F-DA71B6A3FEDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{7E742BB3-A379-DC4A-8D47-23FDDF719C8F}"/>
   </bookViews>
@@ -31,6 +31,53 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>telephone</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>line_id</t>
+  </si>
+  <si>
+    <t>cust_id</t>
+  </si>
+  <si>
+    <t>prod_id</t>
+  </si>
+  <si>
+    <t>prod_name</t>
+  </si>
+  <si>
+    <t>prod_desc</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>invoice_id</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,50 +427,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B986DB-BB36-B84D-86D1-A6D28B854D7C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04174DA-B418-B54F-B1E7-9F87AC115D23}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362C9F12-1435-1B41-B9C0-226C20D5000B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8205A0-83D2-424D-8D3F-F974D2D2C40A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04174DA-B418-B54F-B1E7-9F87AC115D23}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362C9F12-1435-1B41-B9C0-226C20D5000B}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8205A0-83D2-424D-8D3F-F974D2D2C40A}">
+  <dimension ref="A2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>